<commit_message>
Added PCA code for more LLMs
</commit_message>
<xml_diff>
--- a/dimension_reduction/PrincipalComponentAnalysis_results.xlsx
+++ b/dimension_reduction/PrincipalComponentAnalysis_results.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasmuskrebs/Documents/School/master_thesis/repo/dimension_reduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D9E045F-02FE-224F-9487-66A428669B47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6B4F683-B9EB-9D40-81AE-91C830538CCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19980" xr2:uid="{C8214493-C4A5-054C-B17C-3B65FE6FA079}"/>
+    <workbookView xWindow="26820" yWindow="940" windowWidth="19200" windowHeight="19860" xr2:uid="{C8214493-C4A5-054C-B17C-3B65FE6FA079}"/>
   </bookViews>
   <sheets>
-    <sheet name="Ark1" sheetId="1" r:id="rId1"/>
+    <sheet name="Dimension Reduction" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -74,75 +74,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A24" authorId="0" shapeId="0" xr:uid="{B243B211-C05D-D24E-98F9-8F82D442F9A7}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Rasmus Krebs:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Called on methods, can't be called on class. Also fit_transform have been omitted, as this just calls fit+transform
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S24" authorId="0" shapeId="0" xr:uid="{1E7FC892-145D-4244-937C-7E6C212761B1}">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Rasmus Krebs:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Called on methods, can't be called on class. Also fit_transform have been omitted, as this just calls fit+transform
-</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="V24" authorId="0" shapeId="0" xr:uid="{7025C84F-AB96-0A4E-BD7B-8085AE631777}">
+    <comment ref="A29" authorId="0" shapeId="0" xr:uid="{B243B211-C05D-D24E-98F9-8F82D442F9A7}">
       <text>
         <r>
           <rPr>
@@ -181,7 +113,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="47">
   <si>
     <t>GPT 3.5</t>
   </si>
@@ -304,6 +236,24 @@
   </si>
   <si>
     <t xml:space="preserve">Models </t>
+  </si>
+  <si>
+    <t>Fatal Errors (F)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Errors (E) </t>
+  </si>
+  <si>
+    <t>Warnings (W)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Refactoring Checks (R) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Style Convenetion Errors (C) </t>
+  </si>
+  <si>
+    <t>CPU usage</t>
   </si>
 </sst>
 </file>
@@ -446,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -493,6 +443,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -502,32 +473,8 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -843,10 +790,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FC5125-E804-5749-A55F-8E8CD1C5214E}">
-  <dimension ref="A1:V25"/>
+  <dimension ref="A1:U37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U23" sqref="U23"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -859,31 +807,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="24" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="16"/>
-      <c r="C1" s="27" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" s="2"/>
@@ -891,36 +839,36 @@
       <c r="C2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="17"/>
-      <c r="F2" s="17"/>
-      <c r="G2" s="18" t="s">
+      <c r="D2" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="24"/>
+      <c r="F2" s="24"/>
+      <c r="G2" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="17" t="s">
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="24" t="s">
         <v>36</v>
       </c>
-      <c r="K2" s="17"/>
-      <c r="L2" s="17"/>
-      <c r="M2" s="21" t="s">
+      <c r="K2" s="24"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="26" t="s">
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="21" t="s">
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
     </row>
     <row r="3" spans="1:21" s="15" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="13" t="s">
@@ -930,58 +878,58 @@
         <v>3</v>
       </c>
       <c r="C3" s="14"/>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="F3" s="24" t="s">
+      <c r="F3" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="H3" s="23" t="s">
+      <c r="H3" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="J3" s="22" t="s">
+      <c r="J3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="K3" s="22" t="s">
+      <c r="K3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="25" t="s">
+      <c r="M3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="25" t="s">
+      <c r="N3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="O3" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="P3" s="19" t="s">
+      <c r="P3" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="Q3" s="19" t="s">
+      <c r="Q3" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="R3" s="19" t="s">
+      <c r="R3" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="S3" s="20" t="s">
+      <c r="S3" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="T3" s="20" t="s">
+      <c r="T3" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="U3" s="20" t="s">
+      <c r="U3" s="17" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1653,7 +1601,7 @@
     </row>
     <row r="14" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="10" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="B14" s="10" t="s">
         <v>22</v>
@@ -1662,746 +1610,1023 @@
         <v>17</v>
       </c>
       <c r="D14" s="10">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E14" s="10">
+        <v>8</v>
+      </c>
+      <c r="F14" s="10">
+        <v>16</v>
+      </c>
+      <c r="G14" s="10">
+        <v>15</v>
+      </c>
+      <c r="H14" s="10">
         <v>7</v>
       </c>
-      <c r="F14" s="10">
-        <v>21</v>
-      </c>
-      <c r="G14" s="10">
-        <v>22</v>
-      </c>
-      <c r="H14" s="10">
+      <c r="I14" s="10">
+        <v>11</v>
+      </c>
+      <c r="J14" s="10">
+        <v>6</v>
+      </c>
+      <c r="K14" s="10">
+        <v>11</v>
+      </c>
+      <c r="L14" s="10">
+        <v>16</v>
+      </c>
+      <c r="M14" s="10">
+        <v>8</v>
+      </c>
+      <c r="N14" s="10">
         <v>9</v>
       </c>
-      <c r="I14" s="10">
-        <v>12</v>
-      </c>
-      <c r="J14" s="10">
+      <c r="O14" s="10">
         <v>8</v>
       </c>
-      <c r="K14" s="10">
-        <v>22</v>
-      </c>
-      <c r="L14" s="10">
-        <v>20</v>
-      </c>
-      <c r="M14" s="10">
-        <v>11</v>
-      </c>
-      <c r="N14" s="10">
+      <c r="P14" s="10">
         <v>10</v>
       </c>
-      <c r="O14" s="10">
-        <v>11</v>
-      </c>
-      <c r="P14" s="10">
-        <v>12</v>
-      </c>
       <c r="Q14" s="10">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="R14" s="10">
         <v>11</v>
       </c>
       <c r="S14" s="10">
+        <v>14</v>
+      </c>
+      <c r="T14" s="10">
+        <v>15</v>
+      </c>
+      <c r="U14" s="10">
         <v>12</v>
-      </c>
-      <c r="T14" s="10">
-        <v>38</v>
-      </c>
-      <c r="U14" s="10">
-        <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0</v>
+      </c>
+      <c r="F15" s="10">
+        <v>1</v>
+      </c>
+      <c r="G15" s="10">
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0</v>
+      </c>
+      <c r="J15" s="10">
+        <v>0</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0</v>
+      </c>
+      <c r="M15" s="10">
+        <v>0</v>
+      </c>
+      <c r="N15" s="10">
+        <v>0</v>
+      </c>
+      <c r="O15" s="10">
+        <v>1</v>
+      </c>
+      <c r="P15" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="10">
+        <v>0</v>
+      </c>
+      <c r="R15" s="10">
+        <v>0</v>
+      </c>
+      <c r="S15" s="10">
+        <v>0</v>
+      </c>
+      <c r="T15" s="10">
+        <v>4</v>
+      </c>
+      <c r="U15" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0</v>
+      </c>
+      <c r="D16" s="10">
+        <v>2</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0</v>
+      </c>
+      <c r="F16" s="10">
+        <v>4</v>
+      </c>
+      <c r="G16" s="10">
+        <v>2</v>
+      </c>
+      <c r="H16" s="10">
+        <v>2</v>
+      </c>
+      <c r="I16" s="10">
+        <v>1</v>
+      </c>
+      <c r="J16" s="10">
+        <v>2</v>
+      </c>
+      <c r="K16" s="10">
+        <v>11</v>
+      </c>
+      <c r="L16" s="10">
+        <v>1</v>
+      </c>
+      <c r="M16" s="10">
+        <v>3</v>
+      </c>
+      <c r="N16" s="10">
+        <v>1</v>
+      </c>
+      <c r="O16" s="10">
+        <v>0</v>
+      </c>
+      <c r="P16" s="10">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="10">
+        <v>2</v>
+      </c>
+      <c r="R16" s="10">
+        <v>0</v>
+      </c>
+      <c r="S16" s="10">
+        <v>0</v>
+      </c>
+      <c r="T16" s="10">
+        <v>8</v>
+      </c>
+      <c r="U16" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="10">
+        <v>0</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="10">
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0</v>
+      </c>
+      <c r="J17" s="10">
+        <v>0</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0</v>
+      </c>
+      <c r="L17" s="10">
+        <v>3</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0</v>
+      </c>
+      <c r="N17" s="10">
+        <v>0</v>
+      </c>
+      <c r="O17" s="10">
+        <v>0</v>
+      </c>
+      <c r="P17" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>0</v>
+      </c>
+      <c r="R17" s="10">
+        <v>0</v>
+      </c>
+      <c r="S17" s="10">
+        <v>0</v>
+      </c>
+      <c r="T17" s="10">
+        <v>13</v>
+      </c>
+      <c r="U17" s="10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="10">
+        <v>0</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0</v>
+      </c>
+      <c r="J18" s="10">
+        <v>0</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0</v>
+      </c>
+      <c r="M18" s="10">
+        <v>0</v>
+      </c>
+      <c r="N18" s="10">
+        <v>0</v>
+      </c>
+      <c r="O18" s="10">
+        <v>0</v>
+      </c>
+      <c r="P18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>0</v>
+      </c>
+      <c r="R18" s="10">
+        <v>0</v>
+      </c>
+      <c r="S18" s="10">
+        <v>0</v>
+      </c>
+      <c r="T18" s="10">
+        <v>0</v>
+      </c>
+      <c r="U18" s="10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C19" s="10">
+        <f>SUM(C14:C18)</f>
+        <v>17</v>
+      </c>
+      <c r="D19" s="10">
+        <f>SUM(D14:D18)</f>
+        <v>14</v>
+      </c>
+      <c r="E19" s="10">
+        <f t="shared" ref="E19:L19" si="0">SUM(E14:E18)</f>
+        <v>8</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="I19" s="10">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="J19" s="10">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="K19" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="L19" s="10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="M19" s="10">
+        <f t="shared" ref="M19" si="1">SUM(M14:M18)</f>
+        <v>11</v>
+      </c>
+      <c r="N19" s="10">
+        <f t="shared" ref="N19" si="2">SUM(N14:N18)</f>
+        <v>10</v>
+      </c>
+      <c r="O19" s="10">
+        <f t="shared" ref="O19" si="3">SUM(O14:O18)</f>
+        <v>9</v>
+      </c>
+      <c r="P19" s="10">
+        <f t="shared" ref="P19" si="4">SUM(P14:P18)</f>
+        <v>12</v>
+      </c>
+      <c r="Q19" s="10">
+        <f t="shared" ref="Q19" si="5">SUM(Q14:Q18)</f>
+        <v>11</v>
+      </c>
+      <c r="R19" s="10">
+        <f t="shared" ref="R19" si="6">SUM(R14:R18)</f>
+        <v>11</v>
+      </c>
+      <c r="S19" s="10">
+        <f t="shared" ref="S19" si="7">SUM(S14:S18)</f>
+        <v>14</v>
+      </c>
+      <c r="T19" s="10">
+        <f t="shared" ref="T19:U19" si="8">SUM(T14:T18)</f>
+        <v>40</v>
+      </c>
+      <c r="U19" s="10">
+        <f t="shared" si="8"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" s="10" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B20" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="10">
-        <f>C14/C4</f>
+      <c r="C20" s="10">
+        <f>C19/C4</f>
         <v>0.13600000000000001</v>
       </c>
-      <c r="D15" s="10">
-        <f>D14/D4</f>
+      <c r="D20" s="10">
+        <f>D19/D4</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="E15" s="10">
-        <f>E14/E4</f>
-        <v>5.1470588235294115E-2</v>
-      </c>
-      <c r="F15" s="10">
-        <f>F14/F4</f>
+      <c r="E20" s="10">
+        <f t="shared" ref="E20:I20" si="9">E19/E4</f>
+        <v>5.8823529411764705E-2</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="9"/>
         <v>0.15107913669064749</v>
       </c>
-      <c r="G15" s="10">
-        <f t="shared" ref="G15:R15" si="0">G14/G4</f>
-        <v>0.7857142857142857</v>
-      </c>
-      <c r="H15" s="10">
-        <f t="shared" si="0"/>
+      <c r="G20" s="10">
+        <f t="shared" si="9"/>
+        <v>0.6071428571428571</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="9"/>
         <v>8.4905660377358486E-2</v>
       </c>
-      <c r="I15" s="10">
-        <f t="shared" si="0"/>
+      <c r="I20" s="10">
+        <f t="shared" si="9"/>
         <v>9.375E-2</v>
       </c>
-      <c r="J15" s="10">
-        <f t="shared" si="0"/>
+      <c r="J20" s="10">
+        <f t="shared" ref="J20:Q20" si="10">J19/J4</f>
         <v>0.11764705882352941</v>
       </c>
-      <c r="K15" s="10">
-        <f t="shared" si="0"/>
+      <c r="K20" s="10">
+        <f t="shared" si="10"/>
         <v>0.21359223300970873</v>
       </c>
-      <c r="L15" s="10">
-        <f t="shared" si="0"/>
+      <c r="L20" s="10">
+        <f t="shared" si="10"/>
         <v>0.17699115044247787</v>
       </c>
-      <c r="M15" s="10">
-        <f t="shared" si="0"/>
+      <c r="M20" s="10">
+        <f t="shared" si="10"/>
         <v>0.27500000000000002</v>
       </c>
-      <c r="N15" s="10">
-        <f t="shared" si="0"/>
+      <c r="N20" s="10">
+        <f t="shared" si="10"/>
         <v>0.125</v>
       </c>
-      <c r="O15" s="10">
-        <f t="shared" si="0"/>
-        <v>0.13580246913580246</v>
-      </c>
-      <c r="P15" s="10">
-        <f t="shared" si="0"/>
+      <c r="O20" s="10">
+        <f t="shared" si="10"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="P20" s="10">
+        <f t="shared" si="10"/>
         <v>0.32432432432432434</v>
       </c>
-      <c r="Q15" s="10">
-        <f t="shared" si="0"/>
+      <c r="Q20" s="10">
+        <f t="shared" si="10"/>
         <v>0.12790697674418605</v>
       </c>
-      <c r="R15" s="10">
-        <f>R14/R4</f>
+      <c r="R20" s="10">
+        <f>R19/R4</f>
         <v>0.13924050632911392</v>
       </c>
-      <c r="S15" s="10">
-        <f t="shared" ref="S15:U15" si="1">S14/S4</f>
-        <v>0.20338983050847459</v>
-      </c>
-      <c r="T15" s="10">
-        <f t="shared" si="1"/>
-        <v>0.17924528301886791</v>
-      </c>
-      <c r="U15" s="10">
-        <f t="shared" si="1"/>
-        <v>0.15748031496062992</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="7" t="s">
+      <c r="S20" s="10">
+        <f t="shared" ref="S20:U20" si="11">S19/S4</f>
+        <v>0.23728813559322035</v>
+      </c>
+      <c r="T20" s="10">
+        <f t="shared" si="11"/>
+        <v>0.18867924528301888</v>
+      </c>
+      <c r="U20" s="10">
+        <f t="shared" si="11"/>
+        <v>0.17322834645669291</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" s="7" customFormat="1" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="7" t="s">
         <v>21</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C16" s="7">
-        <v>51</v>
-      </c>
-      <c r="D16" s="7">
-        <v>8</v>
-      </c>
-      <c r="E16" s="7">
-        <v>35</v>
-      </c>
-      <c r="F16" s="7">
-        <v>32</v>
-      </c>
-      <c r="G16" s="7">
-        <v>8</v>
-      </c>
-      <c r="H16" s="7">
-        <v>26</v>
-      </c>
-      <c r="I16" s="7">
-        <v>32</v>
-      </c>
-      <c r="J16" s="7">
-        <v>17</v>
-      </c>
-      <c r="K16" s="7">
-        <v>47</v>
-      </c>
-      <c r="L16" s="7">
-        <v>38</v>
-      </c>
-      <c r="M16" s="7">
-        <v>14</v>
-      </c>
-      <c r="N16" s="7">
-        <v>17</v>
-      </c>
-      <c r="O16" s="7">
-        <v>23</v>
-      </c>
-      <c r="P16" s="7">
-        <v>14</v>
-      </c>
-      <c r="Q16" s="7">
-        <v>23</v>
-      </c>
-      <c r="R16" s="7">
-        <v>29</v>
-      </c>
-      <c r="S16" s="7">
-        <v>22</v>
-      </c>
-      <c r="T16" s="7">
-        <v>61</v>
-      </c>
-      <c r="U16" s="7">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="17" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="B17" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" s="7">
-        <v>273.24</v>
-      </c>
-      <c r="D17" s="8">
-        <v>22.458839376460801</v>
-      </c>
-      <c r="E17" s="7">
-        <v>164.52</v>
-      </c>
-      <c r="F17" s="7">
-        <v>148.6</v>
-      </c>
-      <c r="G17" s="7">
-        <v>24</v>
-      </c>
-      <c r="H17" s="7">
-        <v>114.2</v>
-      </c>
-      <c r="I17" s="7">
-        <v>150.41</v>
-      </c>
-      <c r="J17" s="7">
-        <v>64.73</v>
-      </c>
-      <c r="K17" s="7">
-        <v>241.08</v>
-      </c>
-      <c r="L17" s="7">
-        <v>182.68</v>
-      </c>
-      <c r="M17" s="7">
-        <v>48.43</v>
-      </c>
-      <c r="N17" s="7">
-        <v>64.73</v>
-      </c>
-      <c r="O17" s="7">
-        <v>97.7</v>
-      </c>
-      <c r="P17" s="7">
-        <v>48.43</v>
-      </c>
-      <c r="Q17" s="7">
-        <v>95.9</v>
-      </c>
-      <c r="R17" s="7">
-        <v>131.18</v>
-      </c>
-      <c r="S17" s="7">
-        <v>85.92</v>
-      </c>
-      <c r="T17" s="7">
-        <v>322.41000000000003</v>
-      </c>
-      <c r="U17" s="7">
-        <v>169.22</v>
-      </c>
-    </row>
-    <row r="18" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="B18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C18" s="7">
-        <v>5.5</v>
-      </c>
-      <c r="D18" s="7">
-        <v>1</v>
-      </c>
-      <c r="E18" s="7">
-        <v>4.24</v>
-      </c>
-      <c r="F18" s="7">
-        <v>4.9400000000000004</v>
-      </c>
-      <c r="G18" s="7">
-        <v>1.5</v>
-      </c>
-      <c r="H18" s="7">
-        <v>3.4</v>
-      </c>
-      <c r="I18" s="7">
-        <v>3.87</v>
-      </c>
-      <c r="J18" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="K18" s="7">
-        <v>7.83</v>
-      </c>
-      <c r="L18" s="7">
-        <v>3.14</v>
-      </c>
-      <c r="M18" s="7">
-        <v>1.69</v>
-      </c>
-      <c r="N18" s="7">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="O18" s="7">
-        <v>2.68</v>
-      </c>
-      <c r="P18" s="7">
-        <v>1.69</v>
-      </c>
-      <c r="Q18" s="7">
-        <v>2.88</v>
-      </c>
-      <c r="R18" s="7">
-        <v>3.35</v>
-      </c>
-      <c r="S18" s="7">
-        <v>1.75</v>
-      </c>
-      <c r="T18" s="7">
-        <v>5.03</v>
-      </c>
-      <c r="U18" s="7">
-        <v>3.6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="7">
-        <v>1498.39</v>
-      </c>
-      <c r="D19" s="7">
-        <v>22.46</v>
-      </c>
-      <c r="E19" s="7">
-        <v>697.03</v>
-      </c>
-      <c r="F19" s="8">
-        <v>734.27561400673198</v>
-      </c>
-      <c r="G19" s="7">
-        <v>36</v>
-      </c>
-      <c r="H19" s="7">
-        <v>388.28</v>
-      </c>
-      <c r="I19" s="7">
-        <v>581.87</v>
-      </c>
-      <c r="J19" s="7">
-        <v>142.4</v>
-      </c>
-      <c r="K19" s="7">
-        <v>1886.68</v>
-      </c>
-      <c r="L19" s="7">
-        <v>572.95000000000005</v>
-      </c>
-      <c r="M19" s="7">
-        <v>81.73</v>
-      </c>
-      <c r="N19" s="7">
-        <v>142.4</v>
-      </c>
-      <c r="O19" s="7">
-        <v>261.7</v>
-      </c>
-      <c r="P19" s="7">
-        <v>81.73</v>
-      </c>
-      <c r="Q19" s="7">
-        <v>276.66000000000003</v>
-      </c>
-      <c r="R19" s="7">
-        <v>439.85</v>
-      </c>
-      <c r="S19" s="7">
-        <v>150.41999999999999</v>
-      </c>
-      <c r="T19" s="7">
-        <v>1622.45</v>
-      </c>
-      <c r="U19" s="7">
-        <v>609.22</v>
-      </c>
-    </row>
-    <row r="20" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" s="7">
-        <v>83.24</v>
-      </c>
-      <c r="D20" s="7">
-        <v>1.25</v>
-      </c>
-      <c r="E20" s="7">
-        <v>38.72</v>
-      </c>
-      <c r="F20" s="7">
-        <v>40.79</v>
-      </c>
-      <c r="G20" s="7">
-        <v>2</v>
-      </c>
-      <c r="H20" s="7">
-        <v>21.57</v>
-      </c>
-      <c r="I20" s="7">
-        <v>32.299999999999997</v>
-      </c>
-      <c r="J20" s="7">
-        <v>7.91</v>
-      </c>
-      <c r="K20" s="7">
-        <v>104.82</v>
-      </c>
-      <c r="L20" s="7">
-        <v>31.83</v>
-      </c>
-      <c r="M20" s="7">
-        <v>4.54</v>
-      </c>
-      <c r="N20" s="7">
-        <v>7.91</v>
-      </c>
-      <c r="O20" s="7">
-        <v>14.54</v>
-      </c>
-      <c r="P20" s="7">
-        <v>4.54</v>
-      </c>
-      <c r="Q20" s="7">
-        <v>15.37</v>
-      </c>
-      <c r="R20" s="7">
-        <v>24.44</v>
-      </c>
-      <c r="S20" s="7">
-        <v>8.36</v>
-      </c>
-      <c r="T20" s="7">
-        <v>90.14</v>
-      </c>
-      <c r="U20" s="7">
-        <v>33.840000000000003</v>
-      </c>
-    </row>
-    <row r="21" spans="1:22" s="7" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="7" t="s">
-        <v>30</v>
       </c>
       <c r="B21" s="7" t="s">
         <v>5</v>
       </c>
       <c r="C21" s="7">
+        <v>51</v>
+      </c>
+      <c r="D21" s="7">
+        <v>8</v>
+      </c>
+      <c r="E21" s="7">
+        <v>35</v>
+      </c>
+      <c r="F21" s="7">
+        <v>32</v>
+      </c>
+      <c r="G21" s="7">
+        <v>8</v>
+      </c>
+      <c r="H21" s="7">
+        <v>26</v>
+      </c>
+      <c r="I21" s="7">
+        <v>32</v>
+      </c>
+      <c r="J21" s="7">
+        <v>17</v>
+      </c>
+      <c r="K21" s="7">
+        <v>47</v>
+      </c>
+      <c r="L21" s="7">
+        <v>38</v>
+      </c>
+      <c r="M21" s="7">
+        <v>14</v>
+      </c>
+      <c r="N21" s="7">
+        <v>17</v>
+      </c>
+      <c r="O21" s="7">
+        <v>23</v>
+      </c>
+      <c r="P21" s="7">
+        <v>14</v>
+      </c>
+      <c r="Q21" s="7">
+        <v>23</v>
+      </c>
+      <c r="R21" s="7">
+        <v>29</v>
+      </c>
+      <c r="S21" s="7">
+        <v>22</v>
+      </c>
+      <c r="T21" s="7">
+        <v>61</v>
+      </c>
+      <c r="U21" s="7">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C22" s="7">
+        <v>273.24</v>
+      </c>
+      <c r="D22" s="8">
+        <v>22.458839376460801</v>
+      </c>
+      <c r="E22" s="7">
+        <v>164.52</v>
+      </c>
+      <c r="F22" s="7">
+        <v>148.6</v>
+      </c>
+      <c r="G22" s="7">
+        <v>24</v>
+      </c>
+      <c r="H22" s="7">
+        <v>114.2</v>
+      </c>
+      <c r="I22" s="7">
+        <v>150.41</v>
+      </c>
+      <c r="J22" s="7">
+        <v>64.73</v>
+      </c>
+      <c r="K22" s="7">
+        <v>241.08</v>
+      </c>
+      <c r="L22" s="7">
+        <v>182.68</v>
+      </c>
+      <c r="M22" s="7">
+        <v>48.43</v>
+      </c>
+      <c r="N22" s="7">
+        <v>64.73</v>
+      </c>
+      <c r="O22" s="7">
+        <v>97.7</v>
+      </c>
+      <c r="P22" s="7">
+        <v>48.43</v>
+      </c>
+      <c r="Q22" s="7">
+        <v>95.9</v>
+      </c>
+      <c r="R22" s="7">
+        <v>131.18</v>
+      </c>
+      <c r="S22" s="7">
+        <v>85.92</v>
+      </c>
+      <c r="T22" s="7">
+        <v>322.41000000000003</v>
+      </c>
+      <c r="U22" s="7">
+        <v>169.22</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C23" s="7">
+        <v>5.5</v>
+      </c>
+      <c r="D23" s="7">
+        <v>1</v>
+      </c>
+      <c r="E23" s="7">
+        <v>4.24</v>
+      </c>
+      <c r="F23" s="7">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="G23" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="H23" s="7">
+        <v>3.4</v>
+      </c>
+      <c r="I23" s="7">
+        <v>3.87</v>
+      </c>
+      <c r="J23" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="K23" s="7">
+        <v>7.83</v>
+      </c>
+      <c r="L23" s="7">
+        <v>3.14</v>
+      </c>
+      <c r="M23" s="7">
+        <v>1.69</v>
+      </c>
+      <c r="N23" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="O23" s="7">
+        <v>2.68</v>
+      </c>
+      <c r="P23" s="7">
+        <v>1.69</v>
+      </c>
+      <c r="Q23" s="7">
+        <v>2.88</v>
+      </c>
+      <c r="R23" s="7">
+        <v>3.35</v>
+      </c>
+      <c r="S23" s="7">
+        <v>1.75</v>
+      </c>
+      <c r="T23" s="7">
+        <v>5.03</v>
+      </c>
+      <c r="U23" s="7">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C24" s="7">
+        <v>1498.39</v>
+      </c>
+      <c r="D24" s="7">
+        <v>22.46</v>
+      </c>
+      <c r="E24" s="7">
+        <v>697.03</v>
+      </c>
+      <c r="F24" s="8">
+        <v>734.27561400673198</v>
+      </c>
+      <c r="G24" s="7">
+        <v>36</v>
+      </c>
+      <c r="H24" s="7">
+        <v>388.28</v>
+      </c>
+      <c r="I24" s="7">
+        <v>581.87</v>
+      </c>
+      <c r="J24" s="7">
+        <v>142.4</v>
+      </c>
+      <c r="K24" s="7">
+        <v>1886.68</v>
+      </c>
+      <c r="L24" s="7">
+        <v>572.95000000000005</v>
+      </c>
+      <c r="M24" s="7">
+        <v>81.73</v>
+      </c>
+      <c r="N24" s="7">
+        <v>142.4</v>
+      </c>
+      <c r="O24" s="7">
+        <v>261.7</v>
+      </c>
+      <c r="P24" s="7">
+        <v>81.73</v>
+      </c>
+      <c r="Q24" s="7">
+        <v>276.66000000000003</v>
+      </c>
+      <c r="R24" s="7">
+        <v>439.85</v>
+      </c>
+      <c r="S24" s="7">
+        <v>150.41999999999999</v>
+      </c>
+      <c r="T24" s="7">
+        <v>1622.45</v>
+      </c>
+      <c r="U24" s="7">
+        <v>609.22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C25" s="7">
+        <v>83.24</v>
+      </c>
+      <c r="D25" s="7">
+        <v>1.25</v>
+      </c>
+      <c r="E25" s="7">
+        <v>38.72</v>
+      </c>
+      <c r="F25" s="7">
+        <v>40.79</v>
+      </c>
+      <c r="G25" s="7">
+        <v>2</v>
+      </c>
+      <c r="H25" s="7">
+        <v>21.57</v>
+      </c>
+      <c r="I25" s="7">
+        <v>32.299999999999997</v>
+      </c>
+      <c r="J25" s="7">
+        <v>7.91</v>
+      </c>
+      <c r="K25" s="7">
+        <v>104.82</v>
+      </c>
+      <c r="L25" s="7">
+        <v>31.83</v>
+      </c>
+      <c r="M25" s="7">
+        <v>4.54</v>
+      </c>
+      <c r="N25" s="7">
+        <v>7.91</v>
+      </c>
+      <c r="O25" s="7">
+        <v>14.54</v>
+      </c>
+      <c r="P25" s="7">
+        <v>4.54</v>
+      </c>
+      <c r="Q25" s="7">
+        <v>15.37</v>
+      </c>
+      <c r="R25" s="7">
+        <v>24.44</v>
+      </c>
+      <c r="S25" s="7">
+        <v>8.36</v>
+      </c>
+      <c r="T25" s="7">
+        <v>90.14</v>
+      </c>
+      <c r="U25" s="7">
+        <v>33.840000000000003</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" s="7" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C26" s="7">
         <v>0.09</v>
       </c>
-      <c r="D21" s="7">
+      <c r="D26" s="7">
         <v>7.0000000000000001E-3</v>
       </c>
-      <c r="E21" s="7">
+      <c r="E26" s="7">
         <v>5.5E-2</v>
       </c>
-      <c r="F21" s="7">
+      <c r="F26" s="7">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="G21" s="7">
+      <c r="G26" s="7">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="H21" s="7">
+      <c r="H26" s="7">
         <v>3.7999999999999999E-2</v>
       </c>
-      <c r="I21" s="7">
+      <c r="I26" s="7">
         <v>0.05</v>
       </c>
-      <c r="J21" s="7">
+      <c r="J26" s="7">
         <v>0.02</v>
       </c>
-      <c r="K21" s="7">
+      <c r="K26" s="7">
         <v>0.08</v>
       </c>
-      <c r="L21" s="7">
+      <c r="L26" s="7">
         <v>0.06</v>
       </c>
-      <c r="M21" s="7">
+      <c r="M26" s="7">
         <v>0.02</v>
       </c>
-      <c r="N21" s="7">
+      <c r="N26" s="7">
         <v>0.02</v>
       </c>
-      <c r="O21" s="7">
+      <c r="O26" s="7">
         <v>3.3000000000000002E-2</v>
       </c>
-      <c r="P21" s="7">
+      <c r="P26" s="7">
         <v>1.6E-2</v>
       </c>
-      <c r="Q21" s="7">
+      <c r="Q26" s="7">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="R21" s="7">
+      <c r="R26" s="7">
         <v>4.2999999999999997E-2</v>
       </c>
-      <c r="S21" s="7">
+      <c r="S26" s="7">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="T21" s="7">
+      <c r="T26" s="7">
         <v>0.1</v>
       </c>
-      <c r="U21" s="7">
+      <c r="U26" s="7">
         <v>5.6000000000000001E-2</v>
       </c>
     </row>
-    <row r="22" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="3" t="s">
+    <row r="27" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B27" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C22" s="3">
+      <c r="C27" s="3">
         <v>3.4</v>
       </c>
-      <c r="D22" s="3">
+      <c r="D27" s="3">
         <v>1</v>
       </c>
-      <c r="E22" s="9">
+      <c r="E27" s="9">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F22" s="9">
+      <c r="F27" s="9">
         <v>3.4</v>
       </c>
-      <c r="G22" s="3">
+      <c r="G27" s="3">
         <v>1</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H27" s="3">
         <v>2</v>
       </c>
-      <c r="I22" s="3">
+      <c r="I27" s="3">
         <v>3.2</v>
       </c>
-      <c r="J22" s="3">
+      <c r="J27" s="3">
         <v>5</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K27" s="3">
         <v>4</v>
       </c>
-      <c r="L22" s="3">
+      <c r="L27" s="3">
         <v>6.25</v>
       </c>
-      <c r="M22" s="3">
+      <c r="M27" s="3">
         <v>2</v>
       </c>
-      <c r="N22" s="3">
+      <c r="N27" s="3">
         <v>2</v>
       </c>
-      <c r="O22" s="3">
+      <c r="O27" s="3">
         <v>3.2</v>
       </c>
-      <c r="P22" s="3">
+      <c r="P27" s="3">
         <v>2</v>
       </c>
-      <c r="Q22" s="3">
+      <c r="Q27" s="3">
         <v>1.6</v>
       </c>
-      <c r="R22" s="3">
+      <c r="R27" s="3">
         <v>2</v>
       </c>
-      <c r="S22" s="3">
+      <c r="S27" s="3">
         <v>1</v>
       </c>
-      <c r="T22" s="3">
+      <c r="T27" s="3">
         <v>2.27</v>
       </c>
-      <c r="U22" s="3">
+      <c r="U27" s="3">
         <v>3</v>
       </c>
     </row>
-    <row r="23" spans="1:22" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3" t="s">
+    <row r="28" spans="1:21" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="3">
+      <c r="C28" s="3">
         <v>66.400000000000006</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D28" s="3">
         <v>89.87</v>
       </c>
-      <c r="E23" s="3">
+      <c r="E28" s="3">
         <v>55.04</v>
       </c>
-      <c r="F23" s="3">
+      <c r="F28" s="3">
         <v>67.099999999999994</v>
       </c>
-      <c r="G23" s="3">
+      <c r="G28" s="3">
         <v>88.89</v>
       </c>
-      <c r="H23" s="3">
+      <c r="H28" s="3">
         <v>65.19</v>
       </c>
-      <c r="I23" s="3">
+      <c r="I28" s="3">
         <v>67.569999999999993</v>
       </c>
-      <c r="J23" s="3">
+      <c r="J28" s="3">
         <v>81.599999999999994</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K28" s="3">
         <v>70.540000000000006</v>
       </c>
-      <c r="L23" s="3">
+      <c r="L28" s="3">
         <v>71.760000000000005</v>
       </c>
-      <c r="M23" s="3">
+      <c r="M28" s="3">
         <v>86.78</v>
       </c>
-      <c r="N23" s="3">
+      <c r="N28" s="3">
         <v>76.2</v>
       </c>
-      <c r="O23" s="3">
+      <c r="O28" s="3">
         <v>75.489999999999995</v>
       </c>
-      <c r="P23" s="3">
+      <c r="P28" s="3">
         <v>83.38</v>
       </c>
-      <c r="Q23" s="3">
+      <c r="Q28" s="3">
         <v>66.91</v>
       </c>
-      <c r="R23" s="3">
+      <c r="R28" s="3">
         <v>75.209999999999994</v>
       </c>
-      <c r="S23" s="3">
+      <c r="S28" s="3">
         <v>80.400000000000006</v>
       </c>
-      <c r="T23" s="3">
+      <c r="T28" s="3">
         <v>51.27</v>
       </c>
-      <c r="U23" s="3">
+      <c r="U28" s="3">
         <v>64.31</v>
       </c>
     </row>
-    <row r="24" spans="1:22" s="11" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="11" t="s">
+    <row r="29" spans="1:21" s="11" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="11" t="s">
+      <c r="B29" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C24" s="11">
-        <f>119.3+135.2+158.2</f>
-        <v>412.7</v>
-      </c>
-      <c r="D24" s="11">
-        <f>AVERAGE(97.5,130.9)</f>
-        <v>114.2</v>
-      </c>
-      <c r="E24" s="11">
-        <f>71.5+88.3+103.8</f>
-        <v>263.60000000000002</v>
-      </c>
-      <c r="F24" s="11">
-        <f>119.4+135.3+150.8</f>
-        <v>405.5</v>
-      </c>
-      <c r="G24" s="11">
-        <f>((96.8+106)+(121.3+813.7))/2</f>
-        <v>568.9</v>
-      </c>
-      <c r="H24" s="11">
-        <f>70.4+86.9+102.4</f>
-        <v>259.70000000000005</v>
-      </c>
-      <c r="I24" s="11">
-        <f>122.1+138.1+145.8</f>
-        <v>406</v>
-      </c>
-      <c r="J24" s="11">
-        <f>94.2</f>
-        <v>94.2</v>
-      </c>
-      <c r="K24" s="11">
-        <f>119.4+128.2+136</f>
-        <v>383.6</v>
-      </c>
-      <c r="L24" s="11">
-        <f>165.4 + 150.6 + 169.6</f>
-        <v>485.6</v>
-      </c>
-      <c r="M24" s="11">
-        <f>73.8+90.3+106.5</f>
-        <v>270.60000000000002</v>
-      </c>
-      <c r="N24" s="11">
-        <f>82.2+91.3+99.4</f>
-        <v>272.89999999999998</v>
-      </c>
-      <c r="O24" s="11">
-        <f>120.2+136.8+160.1</f>
-        <v>417.1</v>
-      </c>
-      <c r="P24" s="11">
-        <v>107</v>
-      </c>
-      <c r="Q24" s="11">
-        <f>105.4</f>
-        <v>105.4</v>
-      </c>
-      <c r="R24" s="11">
-        <f>112.2</f>
-        <v>112.2</v>
-      </c>
-      <c r="S24" s="11">
-        <v>788.6</v>
-      </c>
-      <c r="T24" s="11">
-        <v>147.5</v>
-      </c>
-      <c r="U24" s="11">
-        <v>222.8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="C25" s="1"/>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="C30" s="1"/>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A37" s="26" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
Added reporting module, to automize the reporting
</commit_message>
<xml_diff>
--- a/dimension_reduction/PrincipalComponentAnalysis_results.xlsx
+++ b/dimension_reduction/PrincipalComponentAnalysis_results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rasmuskrebs/Documents/School/master_thesis/repo/dimension_reduction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56389631-F549-6340-8D3B-1D55D52E0284}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C337DC0C-F8F2-3E4E-AB28-FD546D9E3B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="19960" firstSheet="1" activeTab="1" xr2:uid="{C8214493-C4A5-054C-B17C-3B65FE6FA079}"/>
+    <workbookView xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="19960" activeTab="3" xr2:uid="{C8214493-C4A5-054C-B17C-3B65FE6FA079}"/>
   </bookViews>
   <sheets>
     <sheet name="Dimension Reduction" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Additional Information" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -2236,9 +2237,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53FC5125-E804-5749-A55F-8E8CD1C5214E}">
   <dimension ref="A1:AD37"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="Z5" sqref="Z5:Z8"/>
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="85" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="W1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3869,47 +3870,47 @@
         <v>20</v>
       </c>
       <c r="M19" s="10">
-        <f t="shared" ref="M19" si="1">SUM(M14:M18)</f>
+        <f t="shared" ref="M19:S19" si="1">SUM(M14:M18)</f>
         <v>11</v>
       </c>
       <c r="N19" s="10">
-        <f t="shared" ref="N19" si="2">SUM(N14:N18)</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
       <c r="O19" s="10">
-        <f t="shared" ref="O19" si="3">SUM(O14:O18)</f>
+        <f t="shared" si="1"/>
         <v>9</v>
       </c>
       <c r="P19" s="10">
-        <f t="shared" ref="P19" si="4">SUM(P14:P18)</f>
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
       <c r="Q19" s="10">
-        <f t="shared" ref="Q19" si="5">SUM(Q14:Q18)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="R19" s="10">
-        <f t="shared" ref="R19" si="6">SUM(R14:R18)</f>
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
       <c r="S19" s="10">
-        <f t="shared" ref="S19" si="7">SUM(S14:S18)</f>
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
       <c r="T19" s="10">
-        <f t="shared" ref="T19:AD19" si="8">SUM(T14:T18)</f>
+        <f t="shared" ref="T19:AD19" si="2">SUM(T14:T18)</f>
         <v>40</v>
       </c>
       <c r="U19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>22</v>
       </c>
       <c r="V19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>16</v>
       </c>
       <c r="W19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="X19" s="10">
@@ -3917,27 +3918,27 @@
         <v>18</v>
       </c>
       <c r="Y19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="Z19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="AA19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>20</v>
       </c>
       <c r="AB19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="AC19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>19</v>
       </c>
       <c r="AD19" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="2"/>
         <v>18</v>
       </c>
     </row>
@@ -3949,63 +3950,63 @@
         <v>26</v>
       </c>
       <c r="C20" s="10">
-        <f>C19/C4</f>
+        <f t="shared" ref="C20:I20" si="3">C19/C4</f>
         <v>0.13600000000000001</v>
       </c>
       <c r="D20" s="10">
-        <f>D19/D4</f>
+        <f t="shared" si="3"/>
         <v>0.33333333333333331</v>
       </c>
       <c r="E20" s="10">
-        <f t="shared" ref="E20:I20" si="9">E19/E4</f>
+        <f t="shared" si="3"/>
         <v>5.8823529411764705E-2</v>
       </c>
       <c r="F20" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>0.15107913669064749</v>
       </c>
       <c r="G20" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>0.6071428571428571</v>
       </c>
       <c r="H20" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>8.4905660377358486E-2</v>
       </c>
       <c r="I20" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="3"/>
         <v>9.375E-2</v>
       </c>
       <c r="J20" s="10">
-        <f t="shared" ref="J20:Q20" si="10">J19/J4</f>
+        <f t="shared" ref="J20:Q20" si="4">J19/J4</f>
         <v>0.11764705882352941</v>
       </c>
       <c r="K20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.21359223300970873</v>
       </c>
       <c r="L20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.17699115044247787</v>
       </c>
       <c r="M20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.27500000000000002</v>
       </c>
       <c r="N20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.125</v>
       </c>
       <c r="O20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.1111111111111111</v>
       </c>
       <c r="P20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.32432432432432434</v>
       </c>
       <c r="Q20" s="10">
-        <f t="shared" si="10"/>
+        <f t="shared" si="4"/>
         <v>0.12790697674418605</v>
       </c>
       <c r="R20" s="10">
@@ -4013,51 +4014,51 @@
         <v>0.13924050632911392</v>
       </c>
       <c r="S20" s="10">
-        <f t="shared" ref="S20:AD20" si="11">S19/S4</f>
+        <f t="shared" ref="S20:AD20" si="5">S19/S4</f>
         <v>0.23728813559322035</v>
       </c>
       <c r="T20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.18867924528301888</v>
       </c>
       <c r="U20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.17322834645669291</v>
       </c>
       <c r="V20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.53333333333333333</v>
       </c>
       <c r="W20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.21126760563380281</v>
       </c>
       <c r="X20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.21686746987951808</v>
       </c>
       <c r="Y20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.36585365853658536</v>
       </c>
       <c r="Z20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.46341463414634149</v>
       </c>
       <c r="AA20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.3125</v>
       </c>
       <c r="AB20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.45454545454545453</v>
       </c>
       <c r="AC20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.22619047619047619</v>
       </c>
       <c r="AD20" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="5"/>
         <v>0.25</v>
       </c>
     </row>
@@ -4852,8 +4853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DD5F400-409A-0B4A-826F-7E5FE6579C80}">
   <dimension ref="A1:F87"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A18" zoomScale="117" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView showGridLines="0" topLeftCell="A16" zoomScale="117" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6503,7 +6504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84D0DEC6-391A-0147-B4F5-B4ED50B60C04}">
   <dimension ref="A1:L28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A15" zoomScale="110" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="110" workbookViewId="0">
       <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>

</xml_diff>